<commit_message>
28-08-2025(scroll view fixed )
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Production Date</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Principal Amount</t>
-  </si>
-  <si>
-    <t>Total Amount</t>
   </si>
   <si>
     <t>GST Amount</t>
@@ -471,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,20 +494,19 @@
     <col min="16" max="16" width="18.28515625" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
     <col min="18" max="18" width="17.85546875" customWidth="1"/>
-    <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" customWidth="1"/>
-    <col min="21" max="21" width="24.140625" customWidth="1"/>
-    <col min="22" max="22" width="21.140625" customWidth="1"/>
-    <col min="23" max="23" width="20" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="20" max="20" width="24.140625" customWidth="1"/>
+    <col min="21" max="21" width="21.140625" customWidth="1"/>
+    <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -525,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -549,7 +545,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>12</v>
@@ -566,54 +562,51 @@
       <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>17</v>
+      <c r="U1" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="W1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="5" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -621,18 +614,17 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="3" t="s">
-        <v>23</v>
+      <c r="T2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>